<commit_message>
Changed job.sql and tables (updated with country names)
</commit_message>
<xml_diff>
--- a/table_sql/Tables.xlsx
+++ b/table_sql/Tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danny Phan\Downloads\Computer Science Courses\COSC 3380\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danny Phan\Downloads\Database-Website\table_sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DC763B-9A48-4D4D-9B10-E1C385EA0CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A60616-C69B-41DD-959A-ED89779F1B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{1E6D32AE-3DBD-400E-AEF8-DC871989AC24}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1E6D32AE-3DBD-400E-AEF8-DC871989AC24}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="101">
   <si>
     <t>Employee</t>
   </si>
@@ -215,13 +215,133 @@
   </si>
   <si>
     <t>Vacation</t>
+  </si>
+  <si>
+    <t>Taxes</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>BY</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>EG</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>HT</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>KZ</t>
+  </si>
+  <si>
+    <t>MK</t>
+  </si>
+  <si>
+    <t>MX</t>
+  </si>
+  <si>
+    <t>NI</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>UG</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>VE</t>
+  </si>
+  <si>
+    <t>VN</t>
+  </si>
+  <si>
+    <t>XK</t>
+  </si>
+  <si>
+    <t>YE</t>
+  </si>
+  <si>
+    <t>ZA</t>
+  </si>
+  <si>
+    <t>Tax rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,16 +349,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -246,14 +378,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -482,123 +626,123 @@
     <tableColumn id="2" xr3:uid="{04E5E97D-B642-4361-A371-72FBA26BBB1B}" name="First Name" dataDxfId="63"/>
     <tableColumn id="3" xr3:uid="{70412BA3-AD8A-4A62-91DA-3D4BA8B5A543}" name="Last Name" dataDxfId="62"/>
     <tableColumn id="4" xr3:uid="{E7243D31-E97D-4AD8-8B99-2C94012D9928}" name="Address" dataDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{0173281C-CA9F-4E94-8CF1-D2DC0E47969A}" name="Email" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{B4EFEC6F-9000-47AA-8390-E37D1005A1F2}" name="Date of Birth" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{032BC412-1603-4D2F-B04B-4912F6CE10B6}" name="Nationality" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{215CD00A-41C4-4A53-952E-4017268E45EF}" name="Job" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{ED0B564E-8DBD-4F8D-B43B-A00F05E70218}" name="Zip Code" dataDxfId="25"/>
-    <tableColumn id="10" xr3:uid="{5381867A-A0A7-411D-9C8D-48FF9FA5596E}" name="Benefits" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{DA9145BB-36DF-45EB-8357-95ECD89343BD}" name="Sick Leave " dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{85D18BFA-7B06-4F6C-8360-B65588173ADB}" name="Vacation" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{0173281C-CA9F-4E94-8CF1-D2DC0E47969A}" name="Email" dataDxfId="60"/>
+    <tableColumn id="7" xr3:uid="{B4EFEC6F-9000-47AA-8390-E37D1005A1F2}" name="Date of Birth" dataDxfId="59"/>
+    <tableColumn id="8" xr3:uid="{032BC412-1603-4D2F-B04B-4912F6CE10B6}" name="Nationality" dataDxfId="58"/>
+    <tableColumn id="9" xr3:uid="{215CD00A-41C4-4A53-952E-4017268E45EF}" name="Job" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{ED0B564E-8DBD-4F8D-B43B-A00F05E70218}" name="Zip Code" dataDxfId="56"/>
+    <tableColumn id="10" xr3:uid="{5381867A-A0A7-411D-9C8D-48FF9FA5596E}" name="Benefits" dataDxfId="55"/>
+    <tableColumn id="11" xr3:uid="{DA9145BB-36DF-45EB-8357-95ECD89343BD}" name="Sick Leave " dataDxfId="54"/>
+    <tableColumn id="12" xr3:uid="{85D18BFA-7B06-4F6C-8360-B65588173ADB}" name="Vacation" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{70243564-F8F6-41D4-9429-D74ECB4A0486}" name="Table11" displayName="Table11" ref="A17:F18" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{70243564-F8F6-41D4-9429-D74ECB4A0486}" name="Table11" displayName="Table11" ref="A17:F18" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="A17:F18" xr:uid="{70243564-F8F6-41D4-9429-D74ECB4A0486}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{3F02019F-7CEB-4F92-9A05-4FD8DAE15D3E}" name="Flight ID" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{62236534-5942-41A9-B744-975C04FC9548}" name="Pilot" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{774ECC5D-D2E9-496F-9EB8-2594A4CD2405}" name="Copilot" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{EE65D518-C062-46D4-BCCE-5FC732A60FF4}" name="Departure Airport" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{E7E39D5B-54BE-4D55-99CB-DA2FC0E92EB1}" name="Arrival Airport" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{18610CF7-BD10-4E13-A278-917D85C6F3B7}" name="Date" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{3F02019F-7CEB-4F92-9A05-4FD8DAE15D3E}" name="Flight ID" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{62236534-5942-41A9-B744-975C04FC9548}" name="Pilot" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{774ECC5D-D2E9-496F-9EB8-2594A4CD2405}" name="Copilot" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{EE65D518-C062-46D4-BCCE-5FC732A60FF4}" name="Departure Airport" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{E7E39D5B-54BE-4D55-99CB-DA2FC0E92EB1}" name="Arrival Airport" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{18610CF7-BD10-4E13-A278-917D85C6F3B7}" name="Date" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{69FC2EAE-7816-47B9-B8A7-026B994E49BD}" name="Table14" displayName="Table14" ref="N18:O19" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{69FC2EAE-7816-47B9-B8A7-026B994E49BD}" name="Table14" displayName="Table14" ref="N18:O19" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="N18:O19" xr:uid="{69FC2EAE-7816-47B9-B8A7-026B994E49BD}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0338F5EC-1E44-4B58-BAA0-3C1A816CF917}" name="Office Number" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{98ED0112-C9AD-41C9-9477-DC93E7BCD5AA}" name="Airport ID" dataDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{0338F5EC-1E44-4B58-BAA0-3C1A816CF917}" name="Office Number" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{98ED0112-C9AD-41C9-9477-DC93E7BCD5AA}" name="Airport ID" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{D0BA7BF8-1EA7-4F88-8B7D-5973101F5D5C}" name="Table15" displayName="Table15" ref="Q18:S19" insertRow="1" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{D0BA7BF8-1EA7-4F88-8B7D-5973101F5D5C}" name="Table15" displayName="Table15" ref="Q18:S19" insertRow="1" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="Q18:S19" xr:uid="{D0BA7BF8-1EA7-4F88-8B7D-5973101F5D5C}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{B9F98DF1-9ADE-45BC-A957-4F2E127D8E23}" name="Airport ID" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{AF8431B8-B1E7-498D-9AD5-48F1C791206F}" name="Airport Name" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{98338A06-69FC-4096-B91B-92FCFFE1A4CE}" name="Location" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{B9F98DF1-9ADE-45BC-A957-4F2E127D8E23}" name="Airport ID" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{AF8431B8-B1E7-498D-9AD5-48F1C791206F}" name="Airport Name" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{98338A06-69FC-4096-B91B-92FCFFE1A4CE}" name="Location" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{787C95EB-A933-40C8-811A-F8AF8D786F71}" name="Table16" displayName="Table16" ref="A21:E26" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{787C95EB-A933-40C8-811A-F8AF8D786F71}" name="Table16" displayName="Table16" ref="A21:E26" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A21:E26" xr:uid="{787C95EB-A933-40C8-811A-F8AF8D786F71}"/>
   <tableColumns count="5">
-    <tableColumn id="2" xr3:uid="{73B287F9-7FB8-4976-985A-C930DDC26C1C}" name="Position (pk)" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{550FABD6-1956-475E-A98A-A9C36E047AD6}" name="Pay Rate" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{24D8133E-7A80-49CD-A42C-121E8A974CF9}" name="Overtime Pay Rate" dataDxfId="0"/>
-    <tableColumn id="1" xr3:uid="{2259B567-C1BE-40B5-8FDD-020031F2B0C5}" name="Benefits" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{0A584C72-8AD6-41E8-A49F-85A35E5B392E}" name="Sick Leave" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{73B287F9-7FB8-4976-985A-C930DDC26C1C}" name="Position (pk)" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{550FABD6-1956-475E-A98A-A9C36E047AD6}" name="Pay Rate" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{24D8133E-7A80-49CD-A42C-121E8A974CF9}" name="Overtime Pay Rate" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{2259B567-C1BE-40B5-8FDD-020031F2B0C5}" name="Benefits" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{0A584C72-8AD6-41E8-A49F-85A35E5B392E}" name="Sick Leave" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{4DC66D41-F140-4B48-B98E-D1876CE8FE0E}" name="Table17" displayName="Table17" ref="G21:I23" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{4DC66D41-F140-4B48-B98E-D1876CE8FE0E}" name="Table17" displayName="Table17" ref="G21:I23" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="G21:I23" xr:uid="{4DC66D41-F140-4B48-B98E-D1876CE8FE0E}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D118D9D1-A50C-4FD4-919F-3619A5FF0628}" name="Social Security Number" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{03DD83DF-F2ED-43D8-B514-79682E0B82C0}" name="Flight ID" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{4E35AFAA-6E06-4E9E-87CA-1C0352393E5F}" name="Hours" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{D118D9D1-A50C-4FD4-919F-3619A5FF0628}" name="Social Security Number" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{03DD83DF-F2ED-43D8-B514-79682E0B82C0}" name="Flight ID" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{4E35AFAA-6E06-4E9E-87CA-1C0352393E5F}" name="Hours" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{90210978-9B7C-459D-A7BD-82B393BB4F73}" name="Table19" displayName="Table19" ref="A29:F30" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{90210978-9B7C-459D-A7BD-82B393BB4F73}" name="Table19" displayName="Table19" ref="A29:F30" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A29:F30" xr:uid="{90210978-9B7C-459D-A7BD-82B393BB4F73}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{BC2AD516-35BA-44DE-9926-1E767EDE5B3A}" name="Social Security Number" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{8EC01542-E8E0-4431-A093-C830BDE46E8B}" name="Job" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{76FE23E3-3F44-40ED-907E-36C14DCBFACE}" name="Total Hours Worked" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{EAE2544A-C792-4D81-9FF0-0AAAB4E104D1}" name="Overtime Hours" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{69AD37B7-5429-406B-A2B9-16C28507C1E0}" name="Taxes (percentage of salary)" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{E04A42F5-6FA7-4D2A-A0ED-2731E757A159}" name="Monthly Salary" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{BC2AD516-35BA-44DE-9926-1E767EDE5B3A}" name="Social Security Number" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{8EC01542-E8E0-4431-A093-C830BDE46E8B}" name="Job" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{76FE23E3-3F44-40ED-907E-36C14DCBFACE}" name="Total Hours Worked" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{EAE2544A-C792-4D81-9FF0-0AAAB4E104D1}" name="Overtime Hours" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{69AD37B7-5429-406B-A2B9-16C28507C1E0}" name="Taxes (percentage of salary)" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{E04A42F5-6FA7-4D2A-A0ED-2731E757A159}" name="Monthly Salary" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{23A23E9D-DFC6-4648-8622-B26BF086CC6F}" name="Table173" displayName="Table173" ref="K21:P23" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{23A23E9D-DFC6-4648-8622-B26BF086CC6F}" name="Table173" displayName="Table173" ref="K21:P23" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="K21:P23" xr:uid="{23A23E9D-DFC6-4648-8622-B26BF086CC6F}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E8355DE9-8817-47ED-A89B-42A9671E8DE4}" name="Social Security Number" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{9388C6EE-D7BF-42CA-A570-9BBE391576E0}" name="Office ID" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{6B07F66B-3748-4FBA-AF8A-5509FF0978D5}" name="Hours" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{5FF71454-80B4-48C5-8B7D-A6475219CD5F}" name="Date" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{14A8053D-EA39-43B1-8257-D70F2ABC9984}" name="Hour Start" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{6F6DB235-B772-4A7F-A4AE-F0B1E4CD1763}" name="Hour End" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{E8355DE9-8817-47ED-A89B-42A9671E8DE4}" name="Social Security Number" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{9388C6EE-D7BF-42CA-A570-9BBE391576E0}" name="Office ID" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{6B07F66B-3748-4FBA-AF8A-5509FF0978D5}" name="Hours" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{5FF71454-80B4-48C5-8B7D-A6475219CD5F}" name="Date" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{14A8053D-EA39-43B1-8257-D70F2ABC9984}" name="Hour Start" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{6F6DB235-B772-4A7F-A4AE-F0B1E4CD1763}" name="Hour End" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{324F9B6F-E1AE-4510-9B43-80AAC3D6195E}" name="Table3" displayName="Table3" ref="G17:L18" insertRow="1" totalsRowShown="0" headerRowDxfId="12" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{324F9B6F-E1AE-4510-9B43-80AAC3D6195E}" name="Table3" displayName="Table3" ref="G17:L18" insertRow="1" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="G17:L18" xr:uid="{324F9B6F-E1AE-4510-9B43-80AAC3D6195E}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{16D3479A-014A-4578-99C2-CE4842CFB568}" name="Hour Departure" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{9EEE9DE6-271D-4A85-B057-FB461E7DB0DA}" name="Hour Arrival" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{CA9B0A0B-0D68-49A8-ADA3-98AA72DA5011}" name="Crew member 1" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{2CFFCFB7-2266-436E-94D5-E2A93919496A}" name="2" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{24DC3163-F2B7-40AE-AC0E-10D96049A2AB}" name="3" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{6106B24F-B2A1-4A49-B2A1-619A33EB8960}" name="4" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{16D3479A-014A-4578-99C2-CE4842CFB568}" name="Hour Departure" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{9EEE9DE6-271D-4A85-B057-FB461E7DB0DA}" name="Hour Arrival" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{CA9B0A0B-0D68-49A8-ADA3-98AA72DA5011}" name="Crew member 1" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{2CFFCFB7-2266-436E-94D5-E2A93919496A}" name="2" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{24DC3163-F2B7-40AE-AC0E-10D96049A2AB}" name="3" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{6106B24F-B2A1-4A49-B2A1-619A33EB8960}" name="4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -901,13 +1045,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC32F36-924E-41CE-A312-8CFF8CD6987C}">
-  <dimension ref="A1:S29"/>
+  <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="18.6328125" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.08984375" style="1" customWidth="1"/>
@@ -927,12 +1071,12 @@
     <col min="17" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="29">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="42" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>58</v>
       </c>
@@ -970,72 +1114,72 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12">
       <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12">
       <c r="B4" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12">
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12">
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12">
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12">
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12">
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12">
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12">
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12">
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12">
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12">
       <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" ht="35" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -1079,7 +1223,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" ht="29">
       <c r="N18" s="1" t="s">
         <v>33</v>
       </c>
@@ -1096,7 +1240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1107,7 +1251,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" ht="29">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1151,37 +1295,40 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" ht="29">
       <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19">
       <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19" ht="18" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19">
       <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="H28" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="29.5" thickBot="1">
       <c r="A29" s="1" t="s">
         <v>58</v>
       </c>
@@ -1199,6 +1346,197 @@
       </c>
       <c r="F29" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="15" thickBot="1">
+      <c r="H30" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="15" thickBot="1">
+      <c r="H31" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="15" thickBot="1">
+      <c r="H32" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" ht="15" thickBot="1">
+      <c r="H33" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" ht="15" thickBot="1">
+      <c r="H34" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="8:8" ht="15" thickBot="1">
+      <c r="H35" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="8:8" ht="15" thickBot="1">
+      <c r="H36" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="8:8" ht="15" thickBot="1">
+      <c r="H37" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="8:8" ht="15" thickBot="1">
+      <c r="H38" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="8:8" ht="15" thickBot="1">
+      <c r="H39" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="8:8" ht="15" thickBot="1">
+      <c r="H40" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="8:8" ht="15" thickBot="1">
+      <c r="H41" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="8:8" ht="15" thickBot="1">
+      <c r="H42" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="8:8" ht="15" thickBot="1">
+      <c r="H43" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="8:8" ht="15" thickBot="1">
+      <c r="H44" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="8:8" ht="15" thickBot="1">
+      <c r="H45" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="8:8" ht="15" thickBot="1">
+      <c r="H46" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="8:8" ht="15" thickBot="1">
+      <c r="H47" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="8:8" ht="15" thickBot="1">
+      <c r="H48" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="8:8" ht="15" thickBot="1">
+      <c r="H49" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="8:8" ht="15" thickBot="1">
+      <c r="H50" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="8:8" ht="15" thickBot="1">
+      <c r="H51" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="8:8" ht="15" thickBot="1">
+      <c r="H52" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="8:8" ht="15" thickBot="1">
+      <c r="H53" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="8:8" ht="15" thickBot="1">
+      <c r="H54" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="8:8" ht="15" thickBot="1">
+      <c r="H55" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="8:8" ht="15" thickBot="1">
+      <c r="H56" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="8:8" ht="15" thickBot="1">
+      <c r="H57" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="8:8" ht="15" thickBot="1">
+      <c r="H58" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="8:8" ht="15" thickBot="1">
+      <c r="H59" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="8:8" ht="15" thickBot="1">
+      <c r="H60" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="8:8" ht="15" thickBot="1">
+      <c r="H61" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="8:8" ht="15" thickBot="1">
+      <c r="H62" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="8:8" ht="15" thickBot="1">
+      <c r="H63" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64" spans="8:8" ht="15" thickBot="1">
+      <c r="H64" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="65" spans="8:8" ht="15" thickBot="1">
+      <c r="H65" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="66" spans="8:8" ht="15" thickBot="1">
+      <c r="H66" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added most sql table columns
</commit_message>
<xml_diff>
--- a/table_sql/Tables.xlsx
+++ b/table_sql/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danny Phan\Downloads\Database-Website\table_sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A60616-C69B-41DD-959A-ED89779F1B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3220DD3D-1FE5-4B5B-9F34-91822F47C2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1E6D32AE-3DBD-400E-AEF8-DC871989AC24}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{1E6D32AE-3DBD-400E-AEF8-DC871989AC24}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="90">
   <si>
     <t>Employee</t>
   </si>
@@ -73,36 +73,6 @@
     <t>Crew Member/Flight Attendant</t>
   </si>
   <si>
-    <t>Sarah</t>
-  </si>
-  <si>
-    <t>Rachael</t>
-  </si>
-  <si>
-    <t>Hammad</t>
-  </si>
-  <si>
-    <t>Van Duong</t>
-  </si>
-  <si>
-    <t>John Murray</t>
-  </si>
-  <si>
-    <t>Muhammad Ahmed</t>
-  </si>
-  <si>
-    <t>Miguel Garcia</t>
-  </si>
-  <si>
-    <t>Chandler Murphy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Susie </t>
-  </si>
-  <si>
-    <t>Hu To</t>
-  </si>
-  <si>
     <t>Taxes (percentage of salary)</t>
   </si>
   <si>
@@ -116,9 +86,6 @@
   </si>
   <si>
     <t>Sick Leave</t>
-  </si>
-  <si>
-    <t>Bill Lancester</t>
   </si>
   <si>
     <t>Hours</t>
@@ -341,7 +308,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,16 +370,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="67">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="64">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -619,130 +577,120 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{E406DD9F-BEFA-405F-819F-C53893576B1A}" name="Table9" displayName="Table9" ref="A2:L14" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{E406DD9F-BEFA-405F-819F-C53893576B1A}" name="Table9" displayName="Table9" ref="A2:L14" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
   <autoFilter ref="A2:L14" xr:uid="{E406DD9F-BEFA-405F-819F-C53893576B1A}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{0751AAE0-3DF6-4317-A038-1CF5AD1AC1D8}" name="Social Security Number" dataDxfId="64"/>
-    <tableColumn id="2" xr3:uid="{04E5E97D-B642-4361-A371-72FBA26BBB1B}" name="First Name" dataDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{70412BA3-AD8A-4A62-91DA-3D4BA8B5A543}" name="Last Name" dataDxfId="62"/>
-    <tableColumn id="4" xr3:uid="{E7243D31-E97D-4AD8-8B99-2C94012D9928}" name="Address" dataDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{0173281C-CA9F-4E94-8CF1-D2DC0E47969A}" name="Email" dataDxfId="60"/>
-    <tableColumn id="7" xr3:uid="{B4EFEC6F-9000-47AA-8390-E37D1005A1F2}" name="Date of Birth" dataDxfId="59"/>
-    <tableColumn id="8" xr3:uid="{032BC412-1603-4D2F-B04B-4912F6CE10B6}" name="Nationality" dataDxfId="58"/>
-    <tableColumn id="9" xr3:uid="{215CD00A-41C4-4A53-952E-4017268E45EF}" name="Job" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{ED0B564E-8DBD-4F8D-B43B-A00F05E70218}" name="Zip Code" dataDxfId="56"/>
-    <tableColumn id="10" xr3:uid="{5381867A-A0A7-411D-9C8D-48FF9FA5596E}" name="Benefits" dataDxfId="55"/>
-    <tableColumn id="11" xr3:uid="{DA9145BB-36DF-45EB-8357-95ECD89343BD}" name="Sick Leave " dataDxfId="54"/>
-    <tableColumn id="12" xr3:uid="{85D18BFA-7B06-4F6C-8360-B65588173ADB}" name="Vacation" dataDxfId="53"/>
+    <tableColumn id="1" xr3:uid="{0751AAE0-3DF6-4317-A038-1CF5AD1AC1D8}" name="Social Security Number" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{04E5E97D-B642-4361-A371-72FBA26BBB1B}" name="First Name" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{70412BA3-AD8A-4A62-91DA-3D4BA8B5A543}" name="Last Name" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{E7243D31-E97D-4AD8-8B99-2C94012D9928}" name="Address" dataDxfId="58"/>
+    <tableColumn id="6" xr3:uid="{0173281C-CA9F-4E94-8CF1-D2DC0E47969A}" name="Email" dataDxfId="57"/>
+    <tableColumn id="7" xr3:uid="{B4EFEC6F-9000-47AA-8390-E37D1005A1F2}" name="Date of Birth" dataDxfId="56"/>
+    <tableColumn id="8" xr3:uid="{032BC412-1603-4D2F-B04B-4912F6CE10B6}" name="Nationality" dataDxfId="55"/>
+    <tableColumn id="9" xr3:uid="{215CD00A-41C4-4A53-952E-4017268E45EF}" name="Job" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{ED0B564E-8DBD-4F8D-B43B-A00F05E70218}" name="Zip Code" dataDxfId="53"/>
+    <tableColumn id="10" xr3:uid="{5381867A-A0A7-411D-9C8D-48FF9FA5596E}" name="Benefits" dataDxfId="52"/>
+    <tableColumn id="11" xr3:uid="{DA9145BB-36DF-45EB-8357-95ECD89343BD}" name="Sick Leave " dataDxfId="51"/>
+    <tableColumn id="12" xr3:uid="{85D18BFA-7B06-4F6C-8360-B65588173ADB}" name="Vacation" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{70243564-F8F6-41D4-9429-D74ECB4A0486}" name="Table11" displayName="Table11" ref="A17:F18" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
-  <autoFilter ref="A17:F18" xr:uid="{70243564-F8F6-41D4-9429-D74ECB4A0486}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{3F02019F-7CEB-4F92-9A05-4FD8DAE15D3E}" name="Flight ID" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{62236534-5942-41A9-B744-975C04FC9548}" name="Pilot" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{774ECC5D-D2E9-496F-9EB8-2594A4CD2405}" name="Copilot" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{EE65D518-C062-46D4-BCCE-5FC732A60FF4}" name="Departure Airport" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{E7E39D5B-54BE-4D55-99CB-DA2FC0E92EB1}" name="Arrival Airport" dataDxfId="46"/>
-    <tableColumn id="6" xr3:uid="{18610CF7-BD10-4E13-A278-917D85C6F3B7}" name="Date" dataDxfId="45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{70243564-F8F6-41D4-9429-D74ECB4A0486}" name="Table11" displayName="Table11" ref="A17:K18" insertRow="1" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+  <autoFilter ref="A17:K18" xr:uid="{70243564-F8F6-41D4-9429-D74ECB4A0486}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{3F02019F-7CEB-4F92-9A05-4FD8DAE15D3E}" name="Flight ID" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{62236534-5942-41A9-B744-975C04FC9548}" name="Pilot" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{774ECC5D-D2E9-496F-9EB8-2594A4CD2405}" name="Copilot" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{EE65D518-C062-46D4-BCCE-5FC732A60FF4}" name="Departure Airport" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{E7E39D5B-54BE-4D55-99CB-DA2FC0E92EB1}" name="Arrival Airport" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{18610CF7-BD10-4E13-A278-917D85C6F3B7}" name="Hour Departure" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{AC3826EC-1BB1-4B57-B2CB-0BF50EC868EB}" name="Hour Arrival" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{E062EE78-F5D2-44E6-A207-DAA4765C05D6}" name="Crew member 1" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{F6DE2F66-770D-45F1-9264-F260DB971A76}" name="2" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{5A1E771F-2D30-4CC7-A0BC-25145AB66F9C}" name="3" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{7F080200-CE1A-4FDC-83AF-62393738C2D0}" name="4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{69FC2EAE-7816-47B9-B8A7-026B994E49BD}" name="Table14" displayName="Table14" ref="N18:O19" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{69FC2EAE-7816-47B9-B8A7-026B994E49BD}" name="Table14" displayName="Table14" ref="N18:O19" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="N18:O19" xr:uid="{69FC2EAE-7816-47B9-B8A7-026B994E49BD}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0338F5EC-1E44-4B58-BAA0-3C1A816CF917}" name="Office Number" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{98ED0112-C9AD-41C9-9477-DC93E7BCD5AA}" name="Airport ID" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{0338F5EC-1E44-4B58-BAA0-3C1A816CF917}" name="Office Number" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{98ED0112-C9AD-41C9-9477-DC93E7BCD5AA}" name="Airport ID" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{D0BA7BF8-1EA7-4F88-8B7D-5973101F5D5C}" name="Table15" displayName="Table15" ref="Q18:S19" insertRow="1" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{D0BA7BF8-1EA7-4F88-8B7D-5973101F5D5C}" name="Table15" displayName="Table15" ref="Q18:S19" insertRow="1" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
   <autoFilter ref="Q18:S19" xr:uid="{D0BA7BF8-1EA7-4F88-8B7D-5973101F5D5C}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{B9F98DF1-9ADE-45BC-A957-4F2E127D8E23}" name="Airport ID" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{AF8431B8-B1E7-498D-9AD5-48F1C791206F}" name="Airport Name" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{98338A06-69FC-4096-B91B-92FCFFE1A4CE}" name="Location" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{B9F98DF1-9ADE-45BC-A957-4F2E127D8E23}" name="Airport ID" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{AF8431B8-B1E7-498D-9AD5-48F1C791206F}" name="Airport Name" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{98338A06-69FC-4096-B91B-92FCFFE1A4CE}" name="Location" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{787C95EB-A933-40C8-811A-F8AF8D786F71}" name="Table16" displayName="Table16" ref="A21:E26" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{787C95EB-A933-40C8-811A-F8AF8D786F71}" name="Table16" displayName="Table16" ref="A21:E26" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A21:E26" xr:uid="{787C95EB-A933-40C8-811A-F8AF8D786F71}"/>
   <tableColumns count="5">
-    <tableColumn id="2" xr3:uid="{73B287F9-7FB8-4976-985A-C930DDC26C1C}" name="Position (pk)" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{550FABD6-1956-475E-A98A-A9C36E047AD6}" name="Pay Rate" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{24D8133E-7A80-49CD-A42C-121E8A974CF9}" name="Overtime Pay Rate" dataDxfId="31"/>
-    <tableColumn id="1" xr3:uid="{2259B567-C1BE-40B5-8FDD-020031F2B0C5}" name="Benefits" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{0A584C72-8AD6-41E8-A49F-85A35E5B392E}" name="Sick Leave" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{73B287F9-7FB8-4976-985A-C930DDC26C1C}" name="Position (pk)" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{550FABD6-1956-475E-A98A-A9C36E047AD6}" name="Pay Rate" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{24D8133E-7A80-49CD-A42C-121E8A974CF9}" name="Overtime Pay Rate" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{2259B567-C1BE-40B5-8FDD-020031F2B0C5}" name="Benefits" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{0A584C72-8AD6-41E8-A49F-85A35E5B392E}" name="Sick Leave" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{4DC66D41-F140-4B48-B98E-D1876CE8FE0E}" name="Table17" displayName="Table17" ref="G21:I23" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{4DC66D41-F140-4B48-B98E-D1876CE8FE0E}" name="Table17" displayName="Table17" ref="G21:I23" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="G21:I23" xr:uid="{4DC66D41-F140-4B48-B98E-D1876CE8FE0E}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D118D9D1-A50C-4FD4-919F-3619A5FF0628}" name="Social Security Number" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{03DD83DF-F2ED-43D8-B514-79682E0B82C0}" name="Flight ID" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{4E35AFAA-6E06-4E9E-87CA-1C0352393E5F}" name="Hours" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{D118D9D1-A50C-4FD4-919F-3619A5FF0628}" name="Social Security Number" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{03DD83DF-F2ED-43D8-B514-79682E0B82C0}" name="Flight ID" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{4E35AFAA-6E06-4E9E-87CA-1C0352393E5F}" name="Hours" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{90210978-9B7C-459D-A7BD-82B393BB4F73}" name="Table19" displayName="Table19" ref="A29:F30" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{90210978-9B7C-459D-A7BD-82B393BB4F73}" name="Table19" displayName="Table19" ref="A29:F30" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A29:F30" xr:uid="{90210978-9B7C-459D-A7BD-82B393BB4F73}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{BC2AD516-35BA-44DE-9926-1E767EDE5B3A}" name="Social Security Number" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{8EC01542-E8E0-4431-A093-C830BDE46E8B}" name="Job" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{76FE23E3-3F44-40ED-907E-36C14DCBFACE}" name="Total Hours Worked" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{EAE2544A-C792-4D81-9FF0-0AAAB4E104D1}" name="Overtime Hours" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{69AD37B7-5429-406B-A2B9-16C28507C1E0}" name="Taxes (percentage of salary)" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{E04A42F5-6FA7-4D2A-A0ED-2731E757A159}" name="Monthly Salary" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{BC2AD516-35BA-44DE-9926-1E767EDE5B3A}" name="Social Security Number" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{8EC01542-E8E0-4431-A093-C830BDE46E8B}" name="Job" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{76FE23E3-3F44-40ED-907E-36C14DCBFACE}" name="Total Hours Worked" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{EAE2544A-C792-4D81-9FF0-0AAAB4E104D1}" name="Overtime Hours" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{69AD37B7-5429-406B-A2B9-16C28507C1E0}" name="Taxes (percentage of salary)" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{E04A42F5-6FA7-4D2A-A0ED-2731E757A159}" name="Monthly Salary" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{23A23E9D-DFC6-4648-8622-B26BF086CC6F}" name="Table173" displayName="Table173" ref="K21:P23" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{23A23E9D-DFC6-4648-8622-B26BF086CC6F}" name="Table173" displayName="Table173" ref="K21:P23" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="K21:P23" xr:uid="{23A23E9D-DFC6-4648-8622-B26BF086CC6F}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E8355DE9-8817-47ED-A89B-42A9671E8DE4}" name="Social Security Number" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{9388C6EE-D7BF-42CA-A570-9BBE391576E0}" name="Office ID" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{6B07F66B-3748-4FBA-AF8A-5509FF0978D5}" name="Hours" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{5FF71454-80B4-48C5-8B7D-A6475219CD5F}" name="Date" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{14A8053D-EA39-43B1-8257-D70F2ABC9984}" name="Hour Start" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{6F6DB235-B772-4A7F-A4AE-F0B1E4CD1763}" name="Hour End" dataDxfId="8"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{324F9B6F-E1AE-4510-9B43-80AAC3D6195E}" name="Table3" displayName="Table3" ref="G17:L18" insertRow="1" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="G17:L18" xr:uid="{324F9B6F-E1AE-4510-9B43-80AAC3D6195E}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{16D3479A-014A-4578-99C2-CE4842CFB568}" name="Hour Departure" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{9EEE9DE6-271D-4A85-B057-FB461E7DB0DA}" name="Hour Arrival" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{CA9B0A0B-0D68-49A8-ADA3-98AA72DA5011}" name="Crew member 1" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{2CFFCFB7-2266-436E-94D5-E2A93919496A}" name="2" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{24DC3163-F2B7-40AE-AC0E-10D96049A2AB}" name="3" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{6106B24F-B2A1-4A49-B2A1-619A33EB8960}" name="4" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E8355DE9-8817-47ED-A89B-42A9671E8DE4}" name="Social Security Number" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{9388C6EE-D7BF-42CA-A570-9BBE391576E0}" name="Office ID" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{6B07F66B-3748-4FBA-AF8A-5509FF0978D5}" name="Hours" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{5FF71454-80B4-48C5-8B7D-A6475219CD5F}" name="Date" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{14A8053D-EA39-43B1-8257-D70F2ABC9984}" name="Hour Start" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{6F6DB235-B772-4A7F-A4AE-F0B1E4CD1763}" name="Hour End" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1048,10 +996,10 @@
   <dimension ref="A1:S66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.6328125" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.08984375" style="1" customWidth="1"/>
@@ -1071,20 +1019,20 @@
     <col min="17" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="42" customHeight="1">
+    <row r="2" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
@@ -1096,92 +1044,32 @@
         <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="B3" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="B4" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="B12" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="B13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="B14" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="35" customHeight="1">
+    <row r="17" spans="1:19" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>10</v>
@@ -1190,359 +1078,356 @@
         <v>11</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="29">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="N18" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" ht="29">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="H21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="M21" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="29">
+    <row r="24" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" ht="18" customHeight="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" ht="29.5" thickBot="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H30" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H31" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H32" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H33" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H34" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H35" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H36" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H37" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H38" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H39" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H40" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I29" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" ht="15" thickBot="1">
-      <c r="H30" s="2" t="s">
+    </row>
+    <row r="41" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H41" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="15" thickBot="1">
-      <c r="H31" s="2" t="s">
+    <row r="42" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H42" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="15" thickBot="1">
-      <c r="H32" s="2" t="s">
+    <row r="43" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H43" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="8:8" ht="15" thickBot="1">
-      <c r="H33" s="2" t="s">
+    <row r="44" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H44" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="8:8" ht="15" thickBot="1">
-      <c r="H34" s="2" t="s">
+    <row r="45" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H45" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="8:8" ht="15" thickBot="1">
-      <c r="H35" s="2" t="s">
+    <row r="46" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H46" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="8:8" ht="15" thickBot="1">
-      <c r="H36" s="2" t="s">
+    <row r="47" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H47" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="8:8" ht="15" thickBot="1">
-      <c r="H37" s="2" t="s">
+    <row r="48" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H48" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="8:8" ht="15" thickBot="1">
-      <c r="H38" s="2" t="s">
+    <row r="49" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H49" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="8:8" ht="15" thickBot="1">
-      <c r="H39" s="2" t="s">
+    <row r="50" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H50" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="8:8" ht="15" thickBot="1">
-      <c r="H40" s="2" t="s">
+    <row r="51" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H51" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="8:8" ht="15" thickBot="1">
-      <c r="H41" s="2" t="s">
+    <row r="52" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H52" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="8:8" ht="15" thickBot="1">
-      <c r="H42" s="2" t="s">
+    <row r="53" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H53" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="8:8" ht="15" thickBot="1">
-      <c r="H43" s="2" t="s">
+    <row r="54" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H54" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="8:8" ht="15" thickBot="1">
-      <c r="H44" s="2" t="s">
+    <row r="55" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H55" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="8:8" ht="15" thickBot="1">
-      <c r="H45" s="2" t="s">
+    <row r="56" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H56" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="8:8" ht="15" thickBot="1">
-      <c r="H46" s="2" t="s">
+    <row r="57" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H57" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="8:8" ht="15" thickBot="1">
-      <c r="H47" s="2" t="s">
+    <row r="58" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H58" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="8:8" ht="15" thickBot="1">
-      <c r="H48" s="2" t="s">
+    <row r="59" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H59" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="8:8" ht="15" thickBot="1">
-      <c r="H49" s="2" t="s">
+    <row r="60" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H60" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="50" spans="8:8" ht="15" thickBot="1">
-      <c r="H50" s="2" t="s">
+    <row r="61" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H61" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="51" spans="8:8" ht="15" thickBot="1">
-      <c r="H51" s="2" t="s">
+    <row r="62" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H62" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="8:8" ht="15" thickBot="1">
-      <c r="H52" s="2" t="s">
+    <row r="63" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H63" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="8:8" ht="15" thickBot="1">
-      <c r="H53" s="2" t="s">
+    <row r="64" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H64" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="8:8" ht="15" thickBot="1">
-      <c r="H54" s="2" t="s">
+    <row r="65" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H65" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="8:8" ht="15" thickBot="1">
-      <c r="H55" s="2" t="s">
+    <row r="66" spans="8:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H66" s="2" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="56" spans="8:8" ht="15" thickBot="1">
-      <c r="H56" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="57" spans="8:8" ht="15" thickBot="1">
-      <c r="H57" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="58" spans="8:8" ht="15" thickBot="1">
-      <c r="H58" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="59" spans="8:8" ht="15" thickBot="1">
-      <c r="H59" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="60" spans="8:8" ht="15" thickBot="1">
-      <c r="H60" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="61" spans="8:8" ht="15" thickBot="1">
-      <c r="H61" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="62" spans="8:8" ht="15" thickBot="1">
-      <c r="H62" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="63" spans="8:8" ht="15" thickBot="1">
-      <c r="H63" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="64" spans="8:8" ht="15" thickBot="1">
-      <c r="H64" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="65" spans="8:8" ht="15" thickBot="1">
-      <c r="H65" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="66" spans="8:8" ht="15" thickBot="1">
-      <c r="H66" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="9">
+  <tableParts count="8">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -1551,7 +1436,6 @@
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
-    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>